<commit_message>
add foreach validator and is_num () helper
</commit_message>
<xml_diff>
--- a/output/cpc-rewritten.xlsx
+++ b/output/cpc-rewritten.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -133,7 +133,7 @@
     <t>flow parameter</t>
   </si>
   <si>
-    <t xml:space="preserve"> generated pose</t>
+    <t>1</t>
   </si>
   <si>
     <t>operation</t>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>flow magnitude</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>conditional</t>
@@ -929,7 +926,7 @@
         <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -995,7 +992,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1006,7 +1003,7 @@
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1039,7 +1036,7 @@
         <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1105,7 +1102,7 @@
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1116,7 +1113,7 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1138,7 +1135,7 @@
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1146,10 +1143,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" t="s">
         <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1157,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -1168,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -1237,7 +1234,7 @@
         <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1248,7 +1245,7 @@
         <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1325,7 +1322,7 @@
         <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1344,10 +1341,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1355,7 +1352,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1366,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C74">
         <v>7</v>
@@ -1391,7 +1388,7 @@
         <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:3">

</xml_diff>

<commit_message>
a more integrated/comprehensive validation functionalities
</commit_message>
<xml_diff>
--- a/output/cpc-rewritten.xlsx
+++ b/output/cpc-rewritten.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatho\Dropbox\Code\Python\docx-sop-parser\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DE1880-D87D-40AB-9FF7-ECA1158E6C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -133,55 +139,58 @@
     <t>flow parameter</t>
   </si>
   <si>
+    <t>generated pose</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>energy minimization</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>receptor residue</t>
+  </si>
+  <si>
+    <t>target criteria</t>
+  </si>
+  <si>
+    <t>lte 5  Å</t>
+  </si>
+  <si>
+    <t>optimization</t>
+  </si>
+  <si>
+    <t>side chain rotamers</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>flow logical parameter</t>
+  </si>
+  <si>
+    <t>lte</t>
+  </si>
+  <si>
+    <t>flow compared value</t>
+  </si>
+  <si>
+    <t>flow operation</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>flow magnitude</t>
+  </si>
+  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>energy minimization</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>receptor residue</t>
-  </si>
-  <si>
-    <t>target criteria</t>
-  </si>
-  <si>
-    <t>lte 5  Å</t>
-  </si>
-  <si>
-    <t>optimization</t>
-  </si>
-  <si>
-    <t>side chain rotamers</t>
-  </si>
-  <si>
-    <t>while</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>flow logical parameter</t>
-  </si>
-  <si>
-    <t>lte</t>
-  </si>
-  <si>
-    <t>flow compared value</t>
-  </si>
-  <si>
-    <t>flow operation</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>flow magnitude</t>
   </si>
   <si>
     <t>conditional</t>
@@ -223,8 +232,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +270,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -307,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,9 +356,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,6 +408,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,14 +601,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -577,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -588,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -599,7 +658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -610,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -621,7 +680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -632,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -643,7 +702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -654,7 +713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -665,7 +724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -676,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -687,7 +746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -698,7 +757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -709,7 +768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -720,7 +779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -731,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -742,7 +801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -753,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -764,7 +823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -775,7 +834,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -786,7 +845,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -797,7 +856,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -808,7 +867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -819,7 +878,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -830,7 +889,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -841,7 +900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -852,7 +911,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -863,7 +922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -874,7 +933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -885,7 +944,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -896,7 +955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -907,7 +966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -918,7 +977,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
@@ -926,10 +985,10 @@
         <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -940,7 +999,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -951,7 +1010,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -962,7 +1021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -973,7 +1032,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -984,7 +1043,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -992,10 +1051,10 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7</v>
       </c>
@@ -1003,10 +1062,10 @@
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1017,7 +1076,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -1028,7 +1087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1036,10 +1095,10 @@
         <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7</v>
       </c>
@@ -1050,7 +1109,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7</v>
       </c>
@@ -1061,7 +1120,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
@@ -1072,7 +1131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7</v>
       </c>
@@ -1083,7 +1142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -1094,7 +1153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -1102,10 +1161,10 @@
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>8</v>
       </c>
@@ -1113,10 +1172,10 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8</v>
       </c>
@@ -1127,7 +1186,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>8</v>
       </c>
@@ -1135,43 +1194,43 @@
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C55">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
@@ -1182,7 +1241,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>8</v>
       </c>
@@ -1193,7 +1252,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1204,7 +1263,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>8</v>
       </c>
@@ -1215,7 +1274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1226,7 +1285,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
@@ -1234,10 +1293,10 @@
         <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9</v>
       </c>
@@ -1245,10 +1304,10 @@
         <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
@@ -1259,7 +1318,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
@@ -1270,7 +1329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9</v>
       </c>
@@ -1281,7 +1340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9</v>
       </c>
@@ -1292,7 +1351,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9</v>
       </c>
@@ -1303,7 +1362,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>10</v>
       </c>
@@ -1314,7 +1373,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>10</v>
       </c>
@@ -1322,10 +1381,10 @@
         <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>10</v>
       </c>
@@ -1336,40 +1395,40 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C74">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>10</v>
       </c>
@@ -1380,7 +1439,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>10</v>
       </c>
@@ -1388,10 +1447,10 @@
         <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>10</v>
       </c>
@@ -1402,7 +1461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>10</v>
       </c>
@@ -1413,7 +1472,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>10</v>
       </c>
@@ -1424,7 +1483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>10</v>
       </c>
@@ -1435,7 +1494,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
make misc error more explanatory, bugfixes
</commit_message>
<xml_diff>
--- a/output/cpc-rewritten.xlsx
+++ b/output/cpc-rewritten.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>if</t>
+  </si>
+  <si>
+    <t>lt</t>
   </si>
   <si>
     <t xml:space="preserve">7 </t>
@@ -1028,7 +1031,7 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1039,7 +1042,7 @@
         <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1116,7 +1119,7 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1138,7 +1141,7 @@
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1146,10 +1149,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1157,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -1168,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -1248,7 +1251,7 @@
         <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1325,7 +1328,7 @@
         <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1344,10 +1347,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1355,7 +1358,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1366,7 +1369,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C74">
         <v>7</v>

</xml_diff>